<commit_message>
code asm fait plus prepa 2
</commit_message>
<xml_diff>
--- a/Tableaux_DUBP_TAZR.xlsx
+++ b/Tableaux_DUBP_TAZR.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="190">
   <si>
     <t xml:space="preserve">Tableau 1 Description des signaux du schéma de la figure 1</t>
   </si>
@@ -538,7 +538,7 @@
     <t xml:space="preserve">PC (9:2)</t>
   </si>
   <si>
-    <t xml:space="preserve">f</t>
+    <t xml:space="preserve">a</t>
   </si>
   <si>
     <t xml:space="preserve">e</t>
@@ -551,9 +551,6 @@
   </si>
   <si>
     <t xml:space="preserve">b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a</t>
   </si>
   <si>
     <t xml:space="preserve">Instruction</t>
@@ -2318,7 +2315,7 @@
   <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2447,35 +2444,35 @@
       <c r="A4" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="B4" s="21" t="n">
-        <v>12</v>
+      <c r="B4" s="21" t="s">
+        <v>152</v>
       </c>
       <c r="C4" s="21" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4" s="21" t="n">
-        <v>10</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="F4" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="21" t="n">
+        <v>7</v>
+      </c>
+      <c r="F4" s="21" t="n">
+        <v>6</v>
+      </c>
+      <c r="G4" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="H4" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="I4" s="21" t="s">
         <v>155</v>
-      </c>
-      <c r="I4" s="21" t="n">
-        <v>6</v>
       </c>
       <c r="J4" s="21" t="s">
         <v>156</v>
       </c>
       <c r="K4" s="21" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="L4" s="21" t="n">
         <v>9</v>
@@ -2510,135 +2507,135 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B5" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="C5" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="D5" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="E5" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="F5" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="G5" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="H5" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="I5" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="J5" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="K5" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="L5" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="M5" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="N5" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="O5" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="P5" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="J5" s="23" t="s">
+      <c r="Q5" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="K5" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="L5" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="M5" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="N5" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="O5" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="P5" s="23" t="s">
+      <c r="R5" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="S5" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="Q5" s="23" t="s">
-        <v>161</v>
-      </c>
-      <c r="R5" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="S5" s="23" t="s">
+      <c r="T5" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="T5" s="23" t="s">
-        <v>169</v>
-      </c>
       <c r="U5" s="23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B6" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="J6" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="K6" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="L6" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="M6" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="N6" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="O6" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="C6" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="F6" s="25" t="s">
+      <c r="P6" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q6" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="G6" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="H6" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="I6" s="25" t="s">
-        <v>160</v>
-      </c>
-      <c r="J6" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="K6" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="L6" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="M6" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="N6" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="O6" s="25" t="s">
+      <c r="R6" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="P6" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q6" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="R6" s="25" t="s">
+      <c r="S6" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="S6" s="25" t="s">
-        <v>169</v>
-      </c>
       <c r="T6" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="U6" s="26"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="26" t="n">
@@ -2689,7 +2686,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="26" t="n">
@@ -2740,7 +2737,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B9" s="26"/>
       <c r="C9" s="26" t="n">
@@ -2791,70 +2788,70 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="28" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B10" s="29"/>
       <c r="C10" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="I10" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="J10" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="K10" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="L10" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="M10" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="N10" s="29" t="s">
         <v>166</v>
       </c>
-      <c r="D10" s="29" t="s">
-        <v>166</v>
-      </c>
-      <c r="E10" s="29" t="s">
+      <c r="O10" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="P10" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="F10" s="29" t="s">
-        <v>165</v>
-      </c>
-      <c r="G10" s="29" t="s">
-        <v>166</v>
-      </c>
-      <c r="H10" s="29" t="s">
-        <v>160</v>
-      </c>
-      <c r="I10" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="J10" s="29" t="s">
-        <v>162</v>
-      </c>
-      <c r="K10" s="29" t="s">
-        <v>166</v>
-      </c>
-      <c r="L10" s="29" t="s">
-        <v>166</v>
-      </c>
-      <c r="M10" s="29" t="s">
-        <v>163</v>
-      </c>
-      <c r="N10" s="29" t="s">
+      <c r="Q10" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="O10" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="P10" s="29" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q10" s="29" t="s">
+      <c r="R10" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="R10" s="29" t="s">
-        <v>169</v>
-      </c>
       <c r="S10" s="29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="T10" s="26" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="U10" s="26" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B11" s="26" t="n">
         <v>3</v>
@@ -2905,7 +2902,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B12" s="26" t="n">
         <v>6</v>
@@ -2956,7 +2953,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B13" s="26" t="n">
         <v>0</v>
@@ -3007,7 +3004,7 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B14" s="26" t="n">
         <v>0</v>
@@ -3058,7 +3055,7 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B15" s="26" t="n">
         <v>0</v>
@@ -3109,72 +3106,72 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="30" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B16" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="G16" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="H16" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="I16" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="J16" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="K16" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="L16" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="M16" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="C16" s="31" t="s">
-        <v>166</v>
-      </c>
-      <c r="D16" s="31" t="s">
+      <c r="N16" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="O16" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="E16" s="31" t="s">
-        <v>165</v>
-      </c>
-      <c r="F16" s="31" t="s">
-        <v>166</v>
-      </c>
-      <c r="G16" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="H16" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="I16" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="J16" s="31" t="s">
-        <v>166</v>
-      </c>
-      <c r="K16" s="31" t="s">
-        <v>166</v>
-      </c>
-      <c r="L16" s="31" t="s">
-        <v>163</v>
-      </c>
-      <c r="M16" s="31" t="s">
+      <c r="P16" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="N16" s="31" t="s">
-        <v>161</v>
-      </c>
-      <c r="O16" s="31" t="s">
-        <v>165</v>
-      </c>
-      <c r="P16" s="31" t="s">
+      <c r="Q16" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="Q16" s="31" t="s">
-        <v>169</v>
-      </c>
       <c r="R16" s="31" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="S16" s="26" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="T16" s="26" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="U16" s="26" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
@@ -3223,7 +3220,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
@@ -3272,72 +3269,72 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="32" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B19" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="F19" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="G19" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="H19" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="I19" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="J19" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="K19" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="L19" s="33" t="s">
         <v>166</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="M19" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="N19" s="33" t="s">
         <v>164</v>
       </c>
-      <c r="D19" s="33" t="s">
-        <v>165</v>
-      </c>
-      <c r="E19" s="33" t="s">
-        <v>166</v>
-      </c>
-      <c r="F19" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="G19" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="H19" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="I19" s="33" t="s">
-        <v>166</v>
-      </c>
-      <c r="J19" s="33" t="s">
-        <v>166</v>
-      </c>
-      <c r="K19" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="L19" s="33" t="s">
+      <c r="O19" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="M19" s="33" t="s">
-        <v>161</v>
-      </c>
-      <c r="N19" s="33" t="s">
-        <v>165</v>
-      </c>
-      <c r="O19" s="33" t="s">
+      <c r="P19" s="33" t="s">
         <v>168</v>
       </c>
-      <c r="P19" s="33" t="s">
-        <v>169</v>
-      </c>
       <c r="Q19" s="33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="R19" s="26" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="S19" s="26" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="T19" s="26" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="U19" s="26" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B20" s="26"/>
       <c r="C20" s="26" t="n">
@@ -3386,7 +3383,7 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="27" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B21" s="26"/>
       <c r="C21" s="26" t="n">
@@ -3435,7 +3432,7 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="34" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B24" s="34"/>
       <c r="C24" s="34"/>
@@ -3460,7 +3457,7 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="34" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B25" s="34"/>
       <c r="C25" s="34"/>
@@ -3485,12 +3482,12 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
debut if/id et if fait
</commit_message>
<xml_diff>
--- a/Tableaux_DUBP_TAZR.xlsx
+++ b/Tableaux_DUBP_TAZR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -165,7 +165,7 @@
     <t xml:space="preserve">EX</t>
   </si>
   <si>
-    <t xml:space="preserve">SIGNAL ID_rs                : std_logic_vector(6 DOWNTO 0);</t>
+    <t xml:space="preserve">SIGNAL ID_rs                : std_logic_vector(5 DOWNTO 0);</t>
   </si>
   <si>
     <t xml:space="preserve">registre ra1 du banc de registres</t>
@@ -263,7 +263,7 @@
     <t xml:space="preserve">signal qui contrôle l’alu à partir de alucon</t>
   </si>
   <si>
-    <t xml:space="preserve">SIGNAL EX_PCBranch          : std_logic;</t>
+    <t xml:space="preserve">SIGNAL EX_PCBranch          : std_logic_vector(31 DOWNTO 0);</t>
   </si>
   <si>
     <t xml:space="preserve">addresse de branchement</t>
@@ -1086,8 +1086,8 @@
   </sheetPr>
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2314,7 +2314,7 @@
   </sheetPr>
   <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>

</xml_diff>